<commit_message>
get dummiesnfrom aguas feo
</commit_message>
<xml_diff>
--- a/aguas_feo.xlsx
+++ b/aguas_feo.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofia/Desktop/séptimo/Laboratorio de aprendizaje estadístico/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D69B37-40C0-094B-90B3-BA0DB17C6A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052FE682-6439-B04F-851D-9F6AC8B15D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="16760" xr2:uid="{6324267F-9BAA-7545-B8E6-2F1526CC3897}"/>
+    <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="16720" activeTab="1" xr2:uid="{6324267F-9BAA-7545-B8E6-2F1526CC3897}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="15">
   <si>
     <t>kahlua</t>
   </si>
@@ -57,6 +59,30 @@
   </si>
   <si>
     <t>cal</t>
+  </si>
+  <si>
+    <t>sabor</t>
+  </si>
+  <si>
+    <t>tamaño</t>
+  </si>
+  <si>
+    <t>calificacion</t>
+  </si>
+  <si>
+    <t>chico</t>
+  </si>
+  <si>
+    <t>grande</t>
+  </si>
+  <si>
+    <t>con</t>
+  </si>
+  <si>
+    <t>sin</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -430,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C0D889-D417-7B4E-B43C-4AD8B168DFBD}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -830,4 +856,513 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2693101-607F-3A4A-8E37-7733042F5BAE}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{897F8BFE-8485-4443-9B45-44922C276C56}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>